<commit_message>
Refactor cheatsheet layout and chip distribution logic
Renamed components and functions for clarity (e.g., Billing to Cheatsheet). Improved chip distribution error handling, added tooltip with algorithm details, and refined UI structure. Minor code cleanups and added safety fallbacks for styles and logic.
</commit_message>
<xml_diff>
--- a/Poker_Chip_Tracker.xlsx
+++ b/Poker_Chip_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianrogg/IdeaProjects/Pokerapp/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF0A3F7-E78B-8941-B8CF-4F6752FA90CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27D7864-A5ED-6445-8C17-DDFD49792582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="55">
   <si>
     <t>5-point chips</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Nikita</t>
+  </si>
+  <si>
+    <t>=IFERROR(AVERAGE(Table27[@[Day 1]:[Day 19]]), "")</t>
   </si>
 </sst>
 </file>
@@ -925,129 +928,6 @@
   </cellStyles>
   <dxfs count="172">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1114,6 +994,129 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3346,10 +3349,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$44:$U$44</c:f>
+              <c:f>Overview!$B$44:$V$44</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3409,6 +3412,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>55.449999999999989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59.449999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3448,10 +3454,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$45:$U$45</c:f>
+              <c:f>Overview!$B$45:$V$45</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3510,6 +3516,9 @@
                   <c:v>-67.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>-64.55</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>-64.55</c:v>
                 </c:pt>
               </c:numCache>
@@ -3550,10 +3559,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$46:$U$46</c:f>
+              <c:f>Overview!$B$46:$V$46</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3612,6 +3621,9 @@
                   <c:v>0.84999999999999964</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>0.84999999999999964</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0.84999999999999964</c:v>
                 </c:pt>
               </c:numCache>
@@ -3652,10 +3664,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$47:$U$47</c:f>
+              <c:f>Overview!$B$47:$V$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3715,6 +3727,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>-46.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-38.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3754,10 +3769,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$48:$U$48</c:f>
+              <c:f>Overview!$B$48:$V$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3817,6 +3832,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>-44.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-46.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3856,10 +3874,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$49:$U$49</c:f>
+              <c:f>Overview!$B$49:$V$49</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3919,6 +3937,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>56.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42.199999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3960,10 +3981,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$50:$U$50</c:f>
+              <c:f>Overview!$B$50:$V$50</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4022,6 +4043,9 @@
                   <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4064,10 +4088,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$51:$U$51</c:f>
+              <c:f>Overview!$B$51:$V$51</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4127,6 +4151,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.799999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4168,10 +4195,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$B$52:$U$52</c:f>
+              <c:f>Overview!$B$52:$V$52</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4230,6 +4257,9 @@
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>10.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -5396,98 +5426,98 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}" name="Table27" displayName="Table27" ref="A1:W10" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}" name="Table27" displayName="Table27" ref="A1:W10" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:W10" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W10">
     <sortCondition descending="1" ref="W1:W10"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{92EF8CB9-CB80-E148-A598-263592A13A8C}" name="SPIELER" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{7813C1CF-1A9B-6046-832A-CC2ECA89FAB6}" name="Day 1 " dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{92EF8CB9-CB80-E148-A598-263592A13A8C}" name="SPIELER" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{7813C1CF-1A9B-6046-832A-CC2ECA89FAB6}" name="Day 1 " dataDxfId="27">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B660C4FA-C14B-004F-B492-5035CEBD7DEF}" name="Day 2 " dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{B660C4FA-C14B-004F-B492-5035CEBD7DEF}" name="Day 2 " dataDxfId="26">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6C4A40C8-4461-204D-B46B-3268E768BF76}" name="Day 3" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{6C4A40C8-4461-204D-B46B-3268E768BF76}" name="Day 3" dataDxfId="25">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{399A3E3E-1727-0D4F-A7B6-EB361603F2DA}" name="Day 4" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{399A3E3E-1727-0D4F-A7B6-EB361603F2DA}" name="Day 4" dataDxfId="24">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{72F7BE65-A228-984D-B729-A3258E48126F}" name="Day 5" dataDxfId="17">
+    <tableColumn id="6" xr3:uid="{72F7BE65-A228-984D-B729-A3258E48126F}" name="Day 5" dataDxfId="23">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A0E7C1BE-EC9C-804A-A04D-1BEC5B3371EE}" name="Day 6" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{A0E7C1BE-EC9C-804A-A04D-1BEC5B3371EE}" name="Day 6" dataDxfId="22">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5AF67BEE-5FB5-B24B-9631-F7CE0DBE78B8}" name="Day 7" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{5AF67BEE-5FB5-B24B-9631-F7CE0DBE78B8}" name="Day 7" dataDxfId="21">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{89090C79-1C04-B341-BE68-3B5E2E234225}" name="Day 8" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{89090C79-1C04-B341-BE68-3B5E2E234225}" name="Day 8" dataDxfId="20">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F382EE00-4228-DE42-840E-5F51A3AB0974}" name="Day 9" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{F382EE00-4228-DE42-840E-5F51A3AB0974}" name="Day 9" dataDxfId="19">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B0182922-281E-024C-BB09-AD769F3B4FB4}" name="Day 10" dataDxfId="12">
+    <tableColumn id="12" xr3:uid="{B0182922-281E-024C-BB09-AD769F3B4FB4}" name="Day 10" dataDxfId="18">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{99A4EB56-D651-4BC2-A5CA-859F1A3F15B0}" name="Day 11" dataDxfId="11">
+    <tableColumn id="14" xr3:uid="{99A4EB56-D651-4BC2-A5CA-859F1A3F15B0}" name="Day 11" dataDxfId="17">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{F9993AEC-803F-4BA7-968D-107436BB462C}" name="Day 12" dataDxfId="10">
+    <tableColumn id="15" xr3:uid="{F9993AEC-803F-4BA7-968D-107436BB462C}" name="Day 12" dataDxfId="16">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A5F9D543-03D6-4394-A34A-49965C66E32F}" name="Day 13" dataDxfId="9">
+    <tableColumn id="16" xr3:uid="{A5F9D543-03D6-4394-A34A-49965C66E32F}" name="Day 13" dataDxfId="15">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{F80688AC-2797-4B24-810A-7953A26A1886}" name="Day 14" dataDxfId="8">
+    <tableColumn id="17" xr3:uid="{F80688AC-2797-4B24-810A-7953A26A1886}" name="Day 14" dataDxfId="14">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{0C41B488-8226-4607-9626-810AA705FB58}" name="Day 15" dataDxfId="7">
+    <tableColumn id="18" xr3:uid="{0C41B488-8226-4607-9626-810AA705FB58}" name="Day 15" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{F83DB11A-8AF7-9442-89F2-CAFCE95DA53F}" name="Day 16" dataDxfId="6">
+    <tableColumn id="22" xr3:uid="{F83DB11A-8AF7-9442-89F2-CAFCE95DA53F}" name="Day 16" dataDxfId="12">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_16[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{8F949639-2CF9-854C-8FBD-732212C46E8C}" name="Day 17" dataDxfId="5">
+    <tableColumn id="23" xr3:uid="{8F949639-2CF9-854C-8FBD-732212C46E8C}" name="Day 17" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_17[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{46A12C53-59A6-0642-9030-B8F98C2A5EB0}" name="Day 18" dataDxfId="4">
+    <tableColumn id="24" xr3:uid="{46A12C53-59A6-0642-9030-B8F98C2A5EB0}" name="Day 18" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_18[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{6596C832-E54B-EF46-86CB-26846218D986}" name="Day 19" dataDxfId="3">
+    <tableColumn id="25" xr3:uid="{6596C832-E54B-EF46-86CB-26846218D986}" name="Day 19" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_19[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{84800F19-5824-E94C-8341-DC81AC34B2C0}" name="Day 20" dataDxfId="2">
+    <tableColumn id="26" xr3:uid="{84800F19-5824-E94C-8341-DC81AC34B2C0}" name="Day 20" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E5EE923F-05E4-6546-B9F0-0B9333029A6A}" name="Σ" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{E5EE923F-05E4-6546-B9F0-0B9333029A6A}" name="Σ" dataDxfId="7">
       <calculatedColumnFormula>SUM(B2:U2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{96EC457F-8EF5-9140-8717-7527BFB349F9}" name="SPIELER2" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{96EC457F-8EF5-9140-8717-7527BFB349F9}" name="SPIELER2" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G7" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G7" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="A1:G7" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
     <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="2">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{8B9ED35C-24C5-6844-B237-43D33B16196A}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{E4DF8B73-C3F7-C348-BBAC-F5854E3538E0}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{0FF71DCD-2492-7143-B294-2EFF6F4A222D}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8579,7 +8609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5389194-3CFE-5849-A7F5-A7C6F5BECF20}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="303" workbookViewId="0">
+    <sheetView zoomScale="194" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -9095,8 +9125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CF54A7-313D-D040-8161-1CFA5FC969B6}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="200" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9138,22 +9168,22 @@
       </c>
       <c r="B2" s="17">
         <f t="shared" ref="B2:B7" si="0">SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</f>
-        <v>0</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G2" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -9162,22 +9192,22 @@
       </c>
       <c r="B3" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-14.1</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -9186,22 +9216,22 @@
       </c>
       <c r="B4" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.3000000000000007</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G4" s="10">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -9210,22 +9240,22 @@
       </c>
       <c r="B5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G5" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -9258,22 +9288,22 @@
       </c>
       <c r="B7" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G7" s="10">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9295,23 +9325,23 @@
       </c>
       <c r="C9" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D9" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E9" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="F9" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G9" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -9331,10 +9361,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:AG52"/>
+  <dimension ref="A1:AH52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K11" zoomScale="200" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V46" sqref="V46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9342,7 +9372,7 @@
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -9428,7 +9458,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
         <v>7</v>
       </c>
@@ -9510,11 +9540,11 @@
       </c>
       <c r="U2" s="42">
         <f>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V2" s="37">
         <f t="shared" ref="V2:V10" si="0">SUM(B2:U2)</f>
-        <v>55.449999999999989</v>
+        <v>59.449999999999989</v>
       </c>
       <c r="W2" s="47" t="s">
         <v>7</v>
@@ -9538,8 +9568,11 @@
          (-SUMIF(Table27[[#This Row],[Day 1 ]:[Day 19]], "&lt;0") / COUNTIF(Table27[[#This Row],[Day 1 ]:[Day 19]], "&lt;0")), "")</f>
         <v>1.2062189591880803</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
         <v>4</v>
       </c>
@@ -9650,7 +9683,7 @@
         <v>0.9212066636650158</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
         <v>11</v>
       </c>
@@ -9732,11 +9765,11 @@
       </c>
       <c r="U4" s="20">
         <f>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V4" s="38">
         <f t="shared" si="0"/>
-        <v>-46.4</v>
+        <v>-38.4</v>
       </c>
       <c r="W4" s="45" t="s">
         <v>11</v>
@@ -9761,7 +9794,7 @@
         <v>0.44103547459252146</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
         <v>6</v>
       </c>
@@ -9843,11 +9876,11 @@
       </c>
       <c r="U5" s="20">
         <f>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>0</v>
+        <v>-1.3000000000000007</v>
       </c>
       <c r="V5" s="38">
         <f t="shared" si="0"/>
-        <v>-44.9</v>
+        <v>-46.2</v>
       </c>
       <c r="W5" s="45" t="s">
         <v>6</v>
@@ -9872,7 +9905,7 @@
         <v>0.53232664631487125</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
         <v>8</v>
       </c>
@@ -9954,11 +9987,11 @@
       </c>
       <c r="U6" s="20">
         <f>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>0</v>
+        <v>-14.1</v>
       </c>
       <c r="V6" s="38">
         <f t="shared" si="0"/>
-        <v>56.3</v>
+        <v>42.199999999999996</v>
       </c>
       <c r="W6" s="45" t="s">
         <v>8</v>
@@ -9983,7 +10016,7 @@
         <v>1.5255555555555553</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
         <v>5</v>
       </c>
@@ -10065,11 +10098,11 @@
       </c>
       <c r="U7" s="20">
         <f>IFERROR(VLOOKUP(Table27[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>0</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="V7" s="38">
         <f t="shared" si="0"/>
-        <v>22.4</v>
+        <v>25.799999999999997</v>
       </c>
       <c r="W7" s="45" t="s">
         <v>5</v>
@@ -10094,7 +10127,7 @@
         <v>0.65852795470629866</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
         <v>22</v>
       </c>
@@ -10205,7 +10238,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
@@ -10316,7 +10349,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>50</v>
       </c>
@@ -10427,7 +10460,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="36"/>
       <c r="C11" s="33"/>
@@ -10437,7 +10470,7 @@
       <c r="G11" s="36"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
@@ -10523,7 +10556,7 @@
       </c>
       <c r="V12" s="34">
         <f>SUM(Table27[Σ])</f>
-        <v>-1.2434497875801753E-14</v>
+        <v>-2.6645352591003757E-14</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
@@ -10705,7 +10738,7 @@
       </c>
       <c r="V44" s="42">
         <f>U44+IFERROR(VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>55.449999999999989</v>
+        <v>59.449999999999989</v>
       </c>
       <c r="W44" s="56"/>
     </row>
@@ -10971,7 +11004,7 @@
       </c>
       <c r="V47" s="38">
         <f>U47+IFERROR(VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>-46.4</v>
+        <v>-38.4</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
@@ -11059,7 +11092,7 @@
       </c>
       <c r="V48" s="38">
         <f>U48+IFERROR(VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>-44.9</v>
+        <v>-46.2</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -11147,7 +11180,7 @@
       </c>
       <c r="V49" s="38">
         <f>U49+IFERROR(VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>56.3</v>
+        <v>42.199999999999996</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -11323,7 +11356,7 @@
       </c>
       <c r="V51" s="38">
         <f>U51+IFERROR(VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_20[[SPIELER]:[WIN / LOSS]],2,FALSE),0)</f>
-        <v>22.4</v>
+        <v>25.799999999999997</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>